<commit_message>
Industry and agriculture electricity demand and large scale solar fixed
</commit_message>
<xml_diff>
--- a/Data/Gemeentes Brabant.xlsx
+++ b/Data/Gemeentes Brabant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Brabant-systeem-integratie-model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD13B7B-B0AE-4BAB-B47D-77540B0534AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597B7AFE-505C-46DB-914E-ACD98547CB95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="2" xr2:uid="{017B8E45-61EE-46C1-A9EB-0E4A60A3B11B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11610" uniqueCount="2901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11611" uniqueCount="2903">
   <si>
     <t>ID</t>
   </si>
@@ -8940,6 +8940,12 @@
   </si>
   <si>
     <t>NoordBrabantTotaal</t>
+  </si>
+  <si>
+    <t>aardgas_landbouw_totaal_m3</t>
+  </si>
+  <si>
+    <t>elektriciteit_landbouw_totaal_kwh</t>
   </si>
 </sst>
 </file>
@@ -43157,7 +43163,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43175,6 +43181,12 @@
       <c r="D1" t="s">
         <v>2899</v>
       </c>
+      <c r="E1" t="s">
+        <v>2901</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2902</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -43618,9 +43630,8 @@
         <f>VLOOKUP(A20,'Energiegebruik industrieper gem'!$A$2:$P$354,5,0)</f>
         <v>262413000</v>
       </c>
-      <c r="E20" t="str">
-        <f>VLOOKUP(A20,'Energiegebruik industrieper gem'!$A$2:$P$354,15,0)</f>
-        <v>?</v>
+      <c r="E20">
+        <v>0</v>
       </c>
       <c r="F20">
         <f>VLOOKUP(A20,'Energiegebruik industrieper gem'!$A$2:$P$354,16,0)</f>
@@ -44666,8 +44677,8 @@
       <c r="D68">
         <v>6862037000</v>
       </c>
-      <c r="E68" t="s">
-        <v>2887</v>
+      <c r="E68">
+        <v>0</v>
       </c>
       <c r="F68">
         <v>946994000</v>

</xml_diff>